<commit_message>
Updating cypress wb fixtures
</commit_message>
<xml_diff>
--- a/backend/cypress/fixtures/test_workbooks/additional-eins-workbook.xlsx
+++ b/backend/cypress/fixtures/test_workbooks/additional-eins-workbook.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.4</t>
+    <t xml:space="preserve">1.1.5</t>
   </si>
   <si>
     <t xml:space="preserve">Section</t>
@@ -452,7 +452,7 @@
   <dimension ref="A1:A1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,12 +466,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Workbook 1.1.5: Undate schema source data (#4689)
* Undating cfda-lookup and cluster-names

* Undating cfda-agencies

* Minor script tweaks

* Updating cypress wb fixtures

* Lint

* Lint
</commit_message>
<xml_diff>
--- a/backend/cypress/fixtures/test_workbooks/additional-eins-workbook.xlsx
+++ b/backend/cypress/fixtures/test_workbooks/additional-eins-workbook.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.4</t>
+    <t xml:space="preserve">1.1.5</t>
   </si>
   <si>
     <t xml:space="preserve">Section</t>
@@ -452,7 +452,7 @@
   <dimension ref="A1:A1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,12 +466,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>